<commit_message>
Oracle, DB2, PostgreSQL, SQL Server, MariaDB, and MySQL dialects.
</commit_message>
<xml_diff>
--- a/proof-of-concept/sql-writer/docs/functions.xlsx
+++ b/proof-of-concept/sql-writer/docs/functions.xlsx
@@ -91,51 +91,10 @@
     <t xml:space="preserve">Derby</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">*1 Since Oracle 11g.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Does not implement DISTINCT.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> sep defaults to NULL.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">*2 Since MySQL 5.5 (at least). sep defaults to a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">comma (','). </t>
-    </r>
+    <t xml:space="preserve">*1 Since Oracle 11g. Does not implement DISTINCT. sep defaults to NULL. Ordering is mandatory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*2 Since MySQL 5.5 (at least). sep defaults to a comma (','). </t>
   </si>
   <si>
     <t xml:space="preserve">*3 Since PostgreSQL 9.0. Does not implement DISTINCT. sep is mandatory.</t>
@@ -506,7 +465,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -541,11 +500,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -614,7 +568,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -641,6 +595,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -743,12 +705,12 @@
   <dimension ref="A1:I74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="G66" activeCellId="0" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.14"/>
@@ -849,7 +811,7 @@
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -860,7 +822,7 @@
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -868,99 +830,99 @@
       <c r="A12" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="D14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10"/>
+      <c r="A16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10"/>
+      <c r="A24" s="12"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
@@ -1033,7 +995,7 @@
       <c r="B28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="13" t="s">
         <v>45</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1059,7 +1021,7 @@
       <c r="B29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="13" t="s">
         <v>47</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1085,13 +1047,13 @@
       <c r="B30" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="13" t="s">
         <v>50</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -1117,7 +1079,7 @@
       <c r="D31" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="13" t="s">
         <v>51</v>
       </c>
       <c r="F31" s="1" t="s">
@@ -1143,7 +1105,7 @@
       <c r="D32" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="13" t="s">
         <v>51</v>
       </c>
       <c r="F32" s="1" t="s">
@@ -1160,22 +1122,22 @@
       <c r="A33" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G33" s="10" t="s">
         <v>43</v>
       </c>
       <c r="H33" s="1" t="s">
@@ -1186,22 +1148,22 @@
       <c r="A34" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="13" t="s">
         <v>45</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G34" s="10" t="s">
         <v>43</v>
       </c>
       <c r="H34" s="1" t="s">
@@ -1212,22 +1174,22 @@
       <c r="A35" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="13" t="s">
         <v>49</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F35" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G35" s="10" t="s">
         <v>43</v>
       </c>
       <c r="H35" s="1" t="s">
@@ -1238,22 +1200,22 @@
       <c r="A36" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G36" s="10" t="s">
         <v>43</v>
       </c>
       <c r="H36" s="1" t="s">
@@ -1334,7 +1296,7 @@
       <c r="E45" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="F45" s="13" t="s">
         <v>71</v>
       </c>
       <c r="G45" s="6" t="s">
@@ -1386,7 +1348,7 @@
       <c r="E47" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F47" s="11" t="s">
+      <c r="F47" s="13" t="s">
         <v>76</v>
       </c>
       <c r="G47" s="1" t="s">
@@ -1403,7 +1365,7 @@
       <c r="B48" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="13" t="s">
         <v>78</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -1412,10 +1374,10 @@
       <c r="E48" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F48" s="11" t="s">
+      <c r="F48" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="11" t="s">
+      <c r="G48" s="13" t="s">
         <v>80</v>
       </c>
       <c r="H48" s="1" t="s">
@@ -1478,10 +1440,10 @@
       <c r="A51" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="13" t="s">
         <v>82</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -1490,10 +1452,10 @@
       <c r="E51" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F51" s="11" t="s">
+      <c r="F51" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="G51" s="11" t="s">
+      <c r="G51" s="13" t="s">
         <v>80</v>
       </c>
       <c r="H51" s="1" t="s">
@@ -1545,7 +1507,7 @@
       <c r="F53" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G53" s="11" t="s">
+      <c r="G53" s="13" t="s">
         <v>83</v>
       </c>
       <c r="H53" s="1" t="s">
@@ -1556,7 +1518,7 @@
       <c r="A54" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="13" t="s">
         <v>84</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -1635,22 +1597,22 @@
       <c r="A63" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="B63" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="C63" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D63" s="11" t="s">
+      <c r="D63" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E63" s="11" t="s">
+      <c r="E63" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="F63" s="11" t="s">
+      <c r="F63" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="G63" s="11" t="s">
+      <c r="G63" s="13" t="s">
         <v>102</v>
       </c>
       <c r="H63" s="6" t="s">
@@ -1664,13 +1626,13 @@
       <c r="A64" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B64" s="11" t="s">
+      <c r="B64" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C64" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D64" s="11" t="s">
+      <c r="D64" s="13" t="s">
         <v>107</v>
       </c>
       <c r="E64" s="6" t="s">
@@ -1693,22 +1655,22 @@
       <c r="A65" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B65" s="11" t="s">
+      <c r="B65" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D65" s="11" t="s">
+      <c r="D65" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E65" s="11" t="s">
+      <c r="E65" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="F65" s="11" t="s">
+      <c r="F65" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="G65" s="11" t="s">
+      <c r="G65" s="13" t="s">
         <v>112</v>
       </c>
       <c r="H65" s="1" t="s">
@@ -1722,25 +1684,25 @@
       <c r="A66" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B66" s="11" t="s">
+      <c r="B66" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C66" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="D66" s="11" t="s">
+      <c r="D66" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="E66" s="11" t="s">
+      <c r="E66" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="F66" s="11" t="s">
+      <c r="F66" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="G66" s="11" t="s">
+      <c r="G66" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="H66" s="11" t="s">
+      <c r="H66" s="13" t="s">
         <v>118</v>
       </c>
       <c r="I66" s="0" t="s">
@@ -1751,13 +1713,13 @@
       <c r="A67" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B67" s="11" t="s">
+      <c r="B67" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C67" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D67" s="11" t="s">
+      <c r="D67" s="13" t="s">
         <v>122</v>
       </c>
       <c r="E67" s="1" t="s">
@@ -1780,10 +1742,10 @@
       <c r="A68" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B68" s="11" t="s">
+      <c r="B68" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="C68" s="13" t="s">
         <v>121</v>
       </c>
       <c r="D68" s="6" t="s">
@@ -1815,19 +1777,19 @@
       <c r="C69" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D69" s="11" t="s">
+      <c r="D69" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E69" s="9" t="s">
+      <c r="E69" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F69" s="9" t="s">
+      <c r="F69" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G69" s="9" t="s">
+      <c r="G69" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H69" s="11" t="s">
+      <c r="H69" s="13" t="s">
         <v>118</v>
       </c>
       <c r="I69" s="0" t="s">
@@ -1838,7 +1800,7 @@
       <c r="A70" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B70" s="10" t="s">
         <v>125</v>
       </c>
       <c r="C70" s="1" t="s">
@@ -1847,13 +1809,13 @@
       <c r="D70" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E70" s="11" t="s">
+      <c r="E70" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="F70" s="11" t="s">
+      <c r="F70" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="G70" s="11" t="s">
+      <c r="G70" s="13" t="s">
         <v>112</v>
       </c>
       <c r="H70" s="1" t="s">
@@ -1867,19 +1829,19 @@
       <c r="A71" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B71" s="11" t="s">
+      <c r="B71" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D71" s="11" t="s">
+      <c r="D71" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E71" s="11" t="s">
+      <c r="E71" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="F71" s="11" t="s">
+      <c r="F71" s="13" t="s">
         <v>129</v>
       </c>
       <c r="G71" s="1" t="s">
@@ -1896,13 +1858,13 @@
       <c r="A72" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B72" s="11" t="s">
+      <c r="B72" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="C72" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D72" s="11" t="s">
+      <c r="D72" s="13" t="s">
         <v>99</v>
       </c>
       <c r="E72" s="1" t="s">
@@ -1911,10 +1873,10 @@
       <c r="F72" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G72" s="9" t="s">
+      <c r="G72" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H72" s="9" t="s">
+      <c r="H72" s="11" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented H2 and HyperSQL dialects.
</commit_message>
<xml_diff>
--- a/proof-of-concept/sql-writer/docs/functions.xlsx
+++ b/proof-of-concept/sql-writer/docs/functions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -218,7 +218,7 @@
     <t xml:space="preserve">log(x) / log(base)</t>
   </si>
   <si>
-    <t xml:space="preserve">trunc(x[, places])</t>
+    <t xml:space="preserve">trunc(x, places)</t>
   </si>
   <si>
     <t xml:space="preserve">exp(p * ln(x))</t>
@@ -272,7 +272,7 @@
     <t xml:space="preserve">upper(x)</t>
   </si>
   <si>
-    <t xml:space="preserve">instr(t, sub [, pos]) *1</t>
+    <t xml:space="preserve">instr(t, sub [, from]) *1</t>
   </si>
   <si>
     <t xml:space="preserve">substr(t, pos [, len]) *2</t>
@@ -284,10 +284,10 @@
     <t xml:space="preserve">concat(x, y)</t>
   </si>
   <si>
-    <t xml:space="preserve">locate(sub, t [, pos]) *1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strpos(t, sub) *3</t>
+    <t xml:space="preserve">locate(sub, t [, from]) *1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strpos(t, from) *3</t>
   </si>
   <si>
     <t xml:space="preserve">x + y , concat(x, y)</t>
@@ -296,7 +296,7 @@
     <t xml:space="preserve">len(x)</t>
   </si>
   <si>
-    <t xml:space="preserve">charindex(sub, t [, pos]) *1</t>
+    <t xml:space="preserve">charindex(sub, t [, from]) *1</t>
   </si>
   <si>
     <t xml:space="preserve">substring(t, pos, len)</t>
@@ -627,12 +627,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -704,33 +704,54 @@
   </sheetPr>
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G66" activeCellId="0" sqref="G66"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A79" activeCellId="0" sqref="A79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
@@ -770,6 +791,11 @@
       <c r="C6" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
+      <c r="G6" s="0"/>
+      <c r="H6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -781,6 +807,11 @@
       <c r="C7" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -792,6 +823,11 @@
       <c r="C8" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+      <c r="G8" s="0"/>
+      <c r="H8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -803,6 +839,11 @@
       <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
+      <c r="G9" s="0"/>
+      <c r="H9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -814,6 +855,11 @@
       <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="D10" s="0"/>
+      <c r="E10" s="0"/>
+      <c r="F10" s="0"/>
+      <c r="G10" s="0"/>
+      <c r="H10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -825,6 +871,11 @@
       <c r="C11" s="9" t="s">
         <v>16</v>
       </c>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
+      <c r="G11" s="0"/>
+      <c r="H11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -840,6 +891,7 @@
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
+      <c r="H12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -851,8 +903,11 @@
       <c r="C13" s="9" t="s">
         <v>20</v>
       </c>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
+      <c r="H13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -865,8 +920,10 @@
         <v>16</v>
       </c>
       <c r="D14" s="10"/>
+      <c r="E14" s="0"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
+      <c r="H14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -882,47 +939,111 @@
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
+      <c r="H15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12"/>
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+      <c r="D16" s="0"/>
+      <c r="E16" s="0"/>
+      <c r="F16" s="0"/>
+      <c r="G16" s="0"/>
+      <c r="H16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
         <v>23</v>
       </c>
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+      <c r="D17" s="0"/>
+      <c r="E17" s="0"/>
+      <c r="F17" s="0"/>
+      <c r="G17" s="0"/>
+      <c r="H17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
         <v>24</v>
       </c>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+      <c r="F18" s="0"/>
+      <c r="G18" s="0"/>
+      <c r="H18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="s">
         <v>25</v>
       </c>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+      <c r="G19" s="0"/>
+      <c r="H19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
         <v>26</v>
       </c>
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0"/>
+      <c r="G20" s="0"/>
+      <c r="H20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
         <v>27</v>
       </c>
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0"/>
+      <c r="G21" s="0"/>
+      <c r="H21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
         <v>28</v>
       </c>
+      <c r="B22" s="0"/>
+      <c r="C22" s="0"/>
+      <c r="D22" s="0"/>
+      <c r="E22" s="0"/>
+      <c r="F22" s="0"/>
+      <c r="G22" s="0"/>
+      <c r="H22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
         <v>29</v>
       </c>
+      <c r="B23" s="0"/>
+      <c r="C23" s="0"/>
+      <c r="D23" s="0"/>
+      <c r="E23" s="0"/>
+      <c r="F23" s="0"/>
+      <c r="G23" s="0"/>
+      <c r="H23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12"/>
+      <c r="B24" s="0"/>
+      <c r="C24" s="0"/>
+      <c r="D24" s="0"/>
+      <c r="E24" s="0"/>
+      <c r="F24" s="0"/>
+      <c r="G24" s="0"/>
+      <c r="H24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
@@ -1144,7 +1265,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>19</v>
       </c>
@@ -1222,25 +1343,71 @@
         <v>44</v>
       </c>
     </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0"/>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="E37" s="0"/>
+      <c r="F37" s="0"/>
+      <c r="G37" s="0"/>
+      <c r="H37" s="0"/>
+    </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>55</v>
       </c>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
+      <c r="F38" s="0"/>
+      <c r="G38" s="0"/>
+      <c r="H38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>56</v>
       </c>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
+      <c r="F39" s="0"/>
+      <c r="G39" s="0"/>
+      <c r="H39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0"/>
+      <c r="F40" s="0"/>
+      <c r="G40" s="0"/>
+      <c r="H40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>58</v>
       </c>
+      <c r="B41" s="0"/>
+      <c r="C41" s="0"/>
+      <c r="D41" s="0"/>
+      <c r="E41" s="0"/>
+      <c r="F41" s="0"/>
+      <c r="G41" s="0"/>
+      <c r="H41" s="0"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0"/>
+      <c r="C42" s="0"/>
+      <c r="D42" s="0"/>
+      <c r="E42" s="0"/>
+      <c r="F42" s="0"/>
+      <c r="G42" s="0"/>
+      <c r="H42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
@@ -1540,20 +1707,68 @@
         <v>73</v>
       </c>
     </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0"/>
+      <c r="C55" s="0"/>
+      <c r="D55" s="0"/>
+      <c r="E55" s="0"/>
+      <c r="F55" s="0"/>
+      <c r="G55" s="0"/>
+      <c r="H55" s="0"/>
+    </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="B56" s="0"/>
+      <c r="C56" s="0"/>
+      <c r="D56" s="0"/>
+      <c r="E56" s="0"/>
+      <c r="F56" s="0"/>
+      <c r="G56" s="0"/>
+      <c r="H56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>86</v>
       </c>
+      <c r="B57" s="0"/>
+      <c r="C57" s="0"/>
+      <c r="D57" s="0"/>
+      <c r="E57" s="0"/>
+      <c r="F57" s="0"/>
+      <c r="G57" s="0"/>
+      <c r="H57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>87</v>
       </c>
+      <c r="B58" s="0"/>
+      <c r="C58" s="0"/>
+      <c r="D58" s="0"/>
+      <c r="E58" s="0"/>
+      <c r="F58" s="0"/>
+      <c r="G58" s="0"/>
+      <c r="H58" s="0"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="0"/>
+      <c r="C59" s="0"/>
+      <c r="D59" s="0"/>
+      <c r="E59" s="0"/>
+      <c r="F59" s="0"/>
+      <c r="G59" s="0"/>
+      <c r="H59" s="0"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="0"/>
+      <c r="C60" s="0"/>
+      <c r="D60" s="0"/>
+      <c r="E60" s="0"/>
+      <c r="F60" s="0"/>
+      <c r="G60" s="0"/>
+      <c r="H60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
@@ -1894,7 +2109,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>